<commit_message>
employment_history_input update to retyr twice instead of once and highlighted mandatory fields on spreadsheet
</commit_message>
<xml_diff>
--- a/employment_history.xlsx
+++ b/employment_history.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elske\PycharmProjects\employmentHeroDataInputAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16C1F14-2453-4912-8BE2-D2ECF3F225C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE81493D-D4CA-4345-B1DB-666B768A4D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39144" yWindow="13368" windowWidth="17280" windowHeight="9960" xr2:uid="{07F0E74D-7CFB-43AE-AEAF-1BF08C4FA094}"/>
+    <workbookView xWindow="35616" yWindow="13548" windowWidth="17280" windowHeight="9960" xr2:uid="{07F0E74D-7CFB-43AE-AEAF-1BF08C4FA094}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,10 +93,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,9 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +470,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,19 +484,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F1" t="s">

</xml_diff>